<commit_message>
Subiendo Calculo de vacaciones por empleado
</commit_message>
<xml_diff>
--- a/Nomina.xlsx
+++ b/Nomina.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgpv3\OneDrive\Escritorio\Ingeniería de Software\PROYECTO\Generacion-Nomina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C598AC2A-26D5-415F-9A57-E854B9133C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F91AEE-91AF-4322-B0EF-87D412A8A3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23820" yWindow="1545" windowWidth="21735" windowHeight="8880" xr2:uid="{D457F33F-D5CB-4BD5-A463-D4BDF7EBF146}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D457F33F-D5CB-4BD5-A463-D4BDF7EBF146}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>EMPLEADO</t>
   </si>
@@ -102,6 +102,48 @@
   </si>
   <si>
     <t>Fecha Ingreso:</t>
+  </si>
+  <si>
+    <t>Lester</t>
+  </si>
+  <si>
+    <t>VACACIONES</t>
+  </si>
+  <si>
+    <t>FechaIngreso:</t>
+  </si>
+  <si>
+    <t>PeriodoInicial</t>
+  </si>
+  <si>
+    <t>PeriodoFinal</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ID_Emp</t>
+  </si>
+  <si>
+    <t>CantDías</t>
+  </si>
+  <si>
+    <t>DiasTomados</t>
+  </si>
+  <si>
+    <t>DiasPendientes</t>
+  </si>
+  <si>
+    <t>SalarioBase_Puesto:</t>
+  </si>
+  <si>
+    <t>SalarioDiario:</t>
+  </si>
+  <si>
+    <t>MontoPagar</t>
+  </si>
+  <si>
+    <t>DíasLaborados</t>
   </si>
 </sst>
 </file>
@@ -174,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -191,11 +233,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -218,9 +269,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -229,9 +277,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -241,13 +286,52 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -584,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7E7709A-0C7A-41F5-94B7-185C2EC665E2}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,29 +687,46 @@
     <col min="10" max="10" width="4.88671875" customWidth="1"/>
     <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5546875" style="9"/>
+    <col min="17" max="17" width="12.5546875" style="9" customWidth="1"/>
+    <col min="18" max="18" width="11.5546875" style="9"/>
+    <col min="19" max="19" width="13.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="14.109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="11" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:23" s="10" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="D1" s="10" t="s">
+      <c r="B1" s="32"/>
+      <c r="D1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="G1" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="K1" s="10" t="s">
+      <c r="E1" s="32"/>
+      <c r="G1" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="K1" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="O1" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -641,67 +742,129 @@
       <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="18">
+      <c r="H2" s="16">
         <v>45627</v>
       </c>
       <c r="K2" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="20">
+      <c r="L2" s="17">
         <v>45627</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="16">
+        <v>42181</v>
+      </c>
+      <c r="R2" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="9">
+        <v>8000</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="V2" s="5">
+        <f>S2/30</f>
+        <v>266.66666666666669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>5750</v>
+        <f>E3</f>
+        <v>5000</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="16">
+        <v>45782</v>
+      </c>
+      <c r="L3" s="17"/>
+      <c r="P3" s="16">
+        <v>45627</v>
+      </c>
+      <c r="S3" s="9">
         <v>5750</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="L3" s="20"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="V3" s="5">
+        <f>S3/30</f>
+        <v>191.66666666666666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5">
         <f>(((E3/30/8)*1.5)*E4)</f>
-        <v>179.6875</v>
+        <v>937.5</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="2">
-        <v>5</v>
-      </c>
-      <c r="G4" s="17">
+        <v>30</v>
+      </c>
+      <c r="G4" s="15">
         <v>45474</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="15">
         <v>45838</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="17">
+      <c r="J4" s="12"/>
+      <c r="K4" s="15">
         <v>45627</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="15">
         <v>45991</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O4" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="T4" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="U4" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="V4" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="W4" s="21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -714,14 +877,47 @@
       <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O5" s="2">
+        <v>1</v>
+      </c>
+      <c r="P5" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="17">
+        <f>+P2</f>
+        <v>42181</v>
+      </c>
+      <c r="R5" s="17">
+        <f>DATE(YEAR(Q5)+1,MONTH(Q5),DAY(Q5))</f>
+        <v>42547</v>
+      </c>
+      <c r="S5" s="9">
+        <f>_xlfn.DAYS(R5,Q5)</f>
+        <v>366</v>
+      </c>
+      <c r="T5" s="5">
+        <f>S5*(15/366)</f>
+        <v>14.999999999999998</v>
+      </c>
+      <c r="U5" s="13">
+        <v>15</v>
+      </c>
+      <c r="V5" s="5">
+        <f t="shared" ref="V5:V15" si="0">T5-U5</f>
+        <v>0</v>
+      </c>
+      <c r="W5" s="25">
+        <f t="shared" ref="W5:W14" si="1">V5*$V$2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="6">
-        <f>+B3+(((B3/30/8)*1.5)*B4)+B5</f>
-        <v>12457.51953125</v>
+        <f>B3+B4+B5</f>
+        <v>6187.5</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
@@ -739,17 +935,50 @@
       <c r="K6" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6" s="2">
         <f>(M4-L2)+1</f>
         <v>365</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O6" s="2">
+        <v>2</v>
+      </c>
+      <c r="P6" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="17">
+        <f>DATE(YEAR(R5),MONTH(R5),DAY(R5))</f>
+        <v>42547</v>
+      </c>
+      <c r="R6" s="17">
+        <f>DATE(YEAR(Q6)+1,MONTH(Q6),DAY(Q6))</f>
+        <v>42912</v>
+      </c>
+      <c r="S6" s="9">
+        <f t="shared" ref="S6:S13" si="2">_xlfn.DAYS(R6,Q6)</f>
+        <v>365</v>
+      </c>
+      <c r="T6" s="5">
+        <f>S6*(15/365)</f>
+        <v>15</v>
+      </c>
+      <c r="U6" s="2">
+        <v>15</v>
+      </c>
+      <c r="V6" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W6" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>4.2999999999999997E-2</v>
+        <v>4.8300000000000003E-2</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -757,77 +986,398 @@
       <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="O7" s="2">
+        <v>3</v>
+      </c>
+      <c r="P7" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="17">
+        <f t="shared" ref="Q7:Q14" si="3">DATE(YEAR(R6),MONTH(R6),DAY(R6))</f>
+        <v>42912</v>
+      </c>
+      <c r="R7" s="17">
+        <f t="shared" ref="R7:R13" si="4">DATE(YEAR(Q7)+1,MONTH(Q7),DAY(Q7))</f>
+        <v>43277</v>
+      </c>
+      <c r="S7" s="9">
+        <f t="shared" si="2"/>
+        <v>365</v>
+      </c>
+      <c r="T7" s="5">
+        <f>S7*(15/365)</f>
+        <v>15</v>
+      </c>
+      <c r="U7" s="2">
+        <v>15</v>
+      </c>
+      <c r="V7" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W7" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.05</v>
-      </c>
       <c r="G8" s="9">
         <v>365</v>
       </c>
       <c r="I8" s="9">
         <f>E3</f>
-        <v>5750</v>
+        <v>5000</v>
       </c>
       <c r="K8" s="9">
         <v>365</v>
       </c>
       <c r="M8" s="9">
         <f>E3</f>
-        <v>5750</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+        <v>5000</v>
+      </c>
+      <c r="O8" s="2">
+        <v>4</v>
+      </c>
+      <c r="P8" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="17">
+        <f t="shared" si="3"/>
+        <v>43277</v>
+      </c>
+      <c r="R8" s="17">
+        <f t="shared" si="4"/>
+        <v>43642</v>
+      </c>
+      <c r="S8" s="9">
+        <f t="shared" si="2"/>
+        <v>365</v>
+      </c>
+      <c r="T8" s="5">
+        <f>S8*(15/365)</f>
+        <v>15</v>
+      </c>
+      <c r="U8" s="2">
+        <v>15</v>
+      </c>
+      <c r="V8" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="4">
         <f>(B7*B3)+(B8*B3)</f>
-        <v>534.75</v>
+        <v>241.5</v>
       </c>
       <c r="G9" s="9">
         <f>H6</f>
         <v>212</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="14">
         <f>(G9*I8)/G8</f>
-        <v>3339.7260273972602</v>
+        <v>2904.1095890410961</v>
       </c>
       <c r="K9" s="9">
         <f>L6</f>
         <v>365</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M9" s="14">
         <f>(K9*M8)/K8</f>
-        <v>5750</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+        <v>5000</v>
+      </c>
+      <c r="O9" s="2">
+        <v>5</v>
+      </c>
+      <c r="P9" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="17">
+        <f t="shared" si="3"/>
+        <v>43642</v>
+      </c>
+      <c r="R9" s="17">
+        <f t="shared" si="4"/>
+        <v>44008</v>
+      </c>
+      <c r="S9" s="9">
+        <f t="shared" si="2"/>
+        <v>366</v>
+      </c>
+      <c r="T9" s="5">
+        <f>S9*(15/366)</f>
+        <v>14.999999999999998</v>
+      </c>
+      <c r="U9" s="2">
+        <v>15</v>
+      </c>
+      <c r="V9" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W9" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="8">
         <f>B6-B9</f>
-        <v>11922.76953125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I11" s="15"/>
-      <c r="M11" s="14"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="H12" s="19"/>
-      <c r="L12" s="19"/>
+        <v>5946</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="10"/>
+      <c r="O10" s="2">
+        <v>6</v>
+      </c>
+      <c r="P10" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="17">
+        <f t="shared" si="3"/>
+        <v>44008</v>
+      </c>
+      <c r="R10" s="17">
+        <f t="shared" si="4"/>
+        <v>44373</v>
+      </c>
+      <c r="S10" s="9">
+        <f t="shared" si="2"/>
+        <v>365</v>
+      </c>
+      <c r="T10" s="5">
+        <f>S10*(15/365)</f>
+        <v>15</v>
+      </c>
+      <c r="U10" s="2">
+        <v>15</v>
+      </c>
+      <c r="V10" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W10" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="20">
+        <f>(I4-H3)+1</f>
+        <v>57</v>
+      </c>
+      <c r="M11" s="13"/>
+      <c r="O11" s="2">
+        <v>7</v>
+      </c>
+      <c r="P11" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="17">
+        <f t="shared" si="3"/>
+        <v>44373</v>
+      </c>
+      <c r="R11" s="17">
+        <f t="shared" si="4"/>
+        <v>44738</v>
+      </c>
+      <c r="S11" s="9">
+        <f t="shared" si="2"/>
+        <v>365</v>
+      </c>
+      <c r="T11" s="5">
+        <f>S11*(15/365)</f>
+        <v>15</v>
+      </c>
+      <c r="U11" s="2">
+        <v>15</v>
+      </c>
+      <c r="V11" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W11" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="L12" s="9"/>
+      <c r="O12" s="2">
+        <v>8</v>
+      </c>
+      <c r="P12" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="17">
+        <f t="shared" si="3"/>
+        <v>44738</v>
+      </c>
+      <c r="R12" s="17">
+        <f t="shared" si="4"/>
+        <v>45103</v>
+      </c>
+      <c r="S12" s="9">
+        <f t="shared" si="2"/>
+        <v>365</v>
+      </c>
+      <c r="T12" s="5">
+        <f>S12*(15/365)</f>
+        <v>15</v>
+      </c>
+      <c r="U12" s="2">
+        <v>15</v>
+      </c>
+      <c r="V12" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W12" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="G13" s="9">
+        <v>365</v>
+      </c>
+      <c r="I13" s="9">
+        <v>7200</v>
+      </c>
+      <c r="O13" s="2">
+        <v>9</v>
+      </c>
+      <c r="P13" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="17">
+        <f t="shared" si="3"/>
+        <v>45103</v>
+      </c>
+      <c r="R13" s="17">
+        <f t="shared" si="4"/>
+        <v>45469</v>
+      </c>
+      <c r="S13" s="9">
+        <f t="shared" si="2"/>
+        <v>366</v>
+      </c>
+      <c r="T13" s="5">
+        <f>S13*(15/366)</f>
+        <v>14.999999999999998</v>
+      </c>
+      <c r="U13" s="2">
+        <v>5</v>
+      </c>
+      <c r="V13" s="5">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999982</v>
+      </c>
+      <c r="W13" s="25">
+        <f t="shared" si="1"/>
+        <v>2666.6666666666665</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="G14" s="9">
+        <f>H11</f>
+        <v>57</v>
+      </c>
+      <c r="I14" s="14">
+        <f>(G14*I13)/G13</f>
+        <v>1124.3835616438357</v>
+      </c>
+      <c r="O14" s="2">
+        <v>10</v>
+      </c>
+      <c r="P14" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="17">
+        <f t="shared" si="3"/>
+        <v>45469</v>
+      </c>
+      <c r="R14" s="17">
+        <v>45791</v>
+      </c>
+      <c r="S14" s="9">
+        <f>_xlfn.DAYS(R14,Q14)</f>
+        <v>322</v>
+      </c>
+      <c r="T14" s="5">
+        <f>S14*(15/365)</f>
+        <v>13.232876712328766</v>
+      </c>
+      <c r="U14" s="2">
+        <v>0</v>
+      </c>
+      <c r="V14" s="5">
+        <f t="shared" si="0"/>
+        <v>13.232876712328766</v>
+      </c>
+      <c r="W14" s="25">
+        <f t="shared" si="1"/>
+        <v>3528.767123287671</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="O15" s="26">
+        <v>11</v>
+      </c>
+      <c r="P15" s="26">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="27">
+        <f>+P3</f>
+        <v>45627</v>
+      </c>
+      <c r="R15" s="28">
+        <v>45791</v>
+      </c>
+      <c r="S15" s="26">
+        <f>_xlfn.DAYS(R15,Q15)</f>
+        <v>164</v>
+      </c>
+      <c r="T15" s="29">
+        <f>S15*(15/365)</f>
+        <v>6.7397260273972597</v>
+      </c>
+      <c r="U15" s="30">
+        <v>1</v>
+      </c>
+      <c r="V15" s="29">
+        <f t="shared" si="0"/>
+        <v>5.7397260273972597</v>
+      </c>
+      <c r="W15" s="31">
+        <f>V15*$V$3</f>
+        <v>1100.1141552511415</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="K1:M1"/>
+    <mergeCell ref="O1:Q1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>